<commit_message>
Switch to single faculty list in FacultyAvailabilityMatrix
</commit_message>
<xml_diff>
--- a/Example3_2020Entry/forBot_FacultyAvailabilityMatrix.xlsx
+++ b/Example3_2020Entry/forBot_FacultyAvailabilityMatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\MCSB Recruitment\2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/github/interviewScheduler/Example3_2020Entry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD3FE84-7B0B-4DA9-825F-E2496F5EE2AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A28C7-A2EE-B849-992D-5A909FFD3724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2600" yWindow="12180" windowWidth="57120" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Ioan Andricioaei</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>Schilling</t>
+  </si>
+  <si>
+    <t>W/ngb/ngd</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -546,6 +549,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,48 +873,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC13"/>
+  <dimension ref="A1:CC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF5" sqref="AF5"/>
+      <pane xSplit="1" topLeftCell="AY1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.875" customWidth="1"/>
-    <col min="3" max="5" width="14.625" customWidth="1"/>
-    <col min="10" max="10" width="17.75" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="3" max="5" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="15" max="15" width="18.875" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="13.875" customWidth="1"/>
-    <col min="22" max="24" width="17.625" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" customWidth="1"/>
+    <col min="22" max="24" width="17.6640625" customWidth="1"/>
     <col min="25" max="26" width="17.5" customWidth="1"/>
     <col min="27" max="27" width="12" customWidth="1"/>
     <col min="30" max="30" width="16.5" customWidth="1"/>
-    <col min="32" max="32" width="14.625" customWidth="1"/>
-    <col min="33" max="33" width="14.125" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
+    <col min="33" max="33" width="14.1640625" customWidth="1"/>
     <col min="39" max="40" width="15.5" customWidth="1"/>
-    <col min="43" max="44" width="15.75" customWidth="1"/>
-    <col min="45" max="45" width="17.75" style="24" customWidth="1"/>
-    <col min="46" max="46" width="12.375" customWidth="1"/>
-    <col min="47" max="47" width="12.875" customWidth="1"/>
-    <col min="48" max="48" width="13.75" customWidth="1"/>
+    <col min="43" max="44" width="15.6640625" customWidth="1"/>
+    <col min="45" max="45" width="17.6640625" style="24" customWidth="1"/>
+    <col min="46" max="46" width="12.33203125" customWidth="1"/>
+    <col min="47" max="47" width="12.83203125" customWidth="1"/>
+    <col min="48" max="48" width="13.6640625" customWidth="1"/>
     <col min="50" max="50" width="14" customWidth="1"/>
     <col min="52" max="52" width="12" customWidth="1"/>
-    <col min="53" max="53" width="9.375" customWidth="1"/>
+    <col min="53" max="53" width="9.33203125" customWidth="1"/>
     <col min="58" max="58" width="13" customWidth="1"/>
-    <col min="60" max="60" width="14.125" customWidth="1"/>
-    <col min="64" max="64" width="13.125" customWidth="1"/>
-    <col min="66" max="66" width="11.875" customWidth="1"/>
+    <col min="60" max="60" width="14.1640625" customWidth="1"/>
+    <col min="64" max="64" width="13.1640625" customWidth="1"/>
+    <col min="66" max="66" width="11.83203125" customWidth="1"/>
     <col min="70" max="70" width="13" customWidth="1"/>
-    <col min="77" max="77" width="17.375" customWidth="1"/>
+    <col min="77" max="77" width="17.33203125" customWidth="1"/>
     <col min="79" max="79" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="26" t="s">
         <v>81</v>
       </c>
@@ -1140,7 +1152,7 @@
       <c r="CB1" s="21"/>
       <c r="CC1" s="21"/>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
@@ -1249,7 +1261,7 @@
       <c r="CB2" s="21"/>
       <c r="CC2" s="21"/>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -1361,7 +1373,7 @@
       <c r="CB3" s="21"/>
       <c r="CC3" s="21"/>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
@@ -1484,7 +1496,7 @@
       <c r="CB4" s="21"/>
       <c r="CC4" s="21"/>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
@@ -1605,7 +1617,7 @@
       <c r="CB5" s="21"/>
       <c r="CC5" s="21"/>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
@@ -1718,7 +1730,7 @@
       <c r="CB6" s="21"/>
       <c r="CC6" s="21"/>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
@@ -1825,7 +1837,7 @@
       <c r="CB7" s="21"/>
       <c r="CC7" s="21"/>
     </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1948,7 +1960,7 @@
       <c r="CB8" s="21"/>
       <c r="CC8" s="21"/>
     </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
@@ -2067,7 +2079,7 @@
       <c r="CB9" s="21"/>
       <c r="CC9" s="21"/>
     </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
@@ -2186,7 +2198,7 @@
       <c r="CB10" s="21"/>
       <c r="CC10" s="21"/>
     </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
@@ -2305,7 +2317,7 @@
       <c r="CB11" s="21"/>
       <c r="CC11" s="21"/>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -2424,7 +2436,7 @@
       <c r="CB12" s="21"/>
       <c r="CC12" s="21"/>
     </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:81" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>70</v>
       </c>
@@ -2537,6 +2549,71 @@
       <c r="CB13" s="21"/>
       <c r="CC13" s="21"/>
     </row>
+    <row r="14" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="U14" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AJ14">
+        <v>1</v>
+      </c>
+      <c r="AK14">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="30">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="30">
+        <v>1</v>
+      </c>
+      <c r="AS14" s="24">
+        <v>1</v>
+      </c>
+      <c r="BC14">
+        <v>1</v>
+      </c>
+      <c r="BD14">
+        <v>1</v>
+      </c>
+      <c r="BM14">
+        <v>1</v>
+      </c>
+      <c r="BN14" s="30">
+        <v>1</v>
+      </c>
+      <c r="BQ14">
+        <v>1</v>
+      </c>
+      <c r="BS14">
+        <v>1</v>
+      </c>
+      <c r="BU14">
+        <v>1</v>
+      </c>
+      <c r="BY14" s="31">
+        <v>1</v>
+      </c>
+      <c r="BZ14">
+        <v>1</v>
+      </c>
+      <c r="CA14" s="30">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2551,9 +2628,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -2561,7 +2638,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2569,12 +2646,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>91</v>
       </c>

</xml_diff>